<commit_message>
Update des monentanen Stand
</commit_message>
<xml_diff>
--- a/src/ASProjekt/Aufgaben.xlsx
+++ b/src/ASProjekt/Aufgaben.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{37D64E56-C126-47CD-BD3D-8246F283F229}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>Aufgabe</t>
   </si>
@@ -85,12 +86,15 @@
   </si>
   <si>
     <t>Optional geplant</t>
+  </si>
+  <si>
+    <t>Leroy | Fixed by Leon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -457,21 +461,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.5546875" customWidth="1"/>
-    <col min="2" max="2" width="28.21875" customWidth="1"/>
-    <col min="3" max="3" width="70.77734375" customWidth="1"/>
+    <col min="1" max="1" width="60.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="70.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -482,7 +486,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -493,7 +497,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -504,7 +508,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -515,18 +519,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -537,7 +541,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -548,7 +552,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -559,18 +563,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C9" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -581,7 +585,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -592,7 +596,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>

</xml_diff>